<commit_message>
fixed dashboard and menu certificate
</commit_message>
<xml_diff>
--- a/frontend/public/data.xlsx
+++ b/frontend/public/data.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6060" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
-    <t>dni</t>
+    <t>DNI</t>
   </si>
   <si>
     <t>name</t>
@@ -132,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,7 +148,7 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -184,11 +185,32 @@
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -200,11 +222,83 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -478,20 +572,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.424285714285714" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.857142857142858" customWidth="1"/>
+    <col min="4" max="4" width="33.714285714285715" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A2">
         <v>548613254</v>
       </c>
@@ -519,7 +613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A3">
         <v>548613255</v>
       </c>
@@ -533,7 +627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A4">
         <v>548613256</v>
       </c>
@@ -547,7 +641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A5">
         <v>548613257</v>
       </c>
@@ -561,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6">
         <v>548613259</v>
       </c>
@@ -575,7 +669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A7">
         <v>548613260</v>
       </c>
@@ -589,7 +683,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A8">
         <v>548613263</v>
       </c>
@@ -603,7 +697,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A9">
         <v>548613264</v>
       </c>
@@ -617,7 +711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A10">
         <v>548613265</v>
       </c>
@@ -631,7 +725,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1" thickBot="1">
       <c r="A11">
         <v>548613266</v>
       </c>
@@ -645,11 +739,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="13.5" customHeight="1">
       <c r="A12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>